<commit_message>
1) Updated EpiQuery data for 2 April 2020. 2) Updated New York State hospitalization data for 2 April 2020.
</commit_message>
<xml_diff>
--- a/data/new_york_state_hospitaliztion_and_discharge.xlsx
+++ b/data/new_york_state_hospitaliztion_and_discharge.xlsx
@@ -147,10 +147,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E19"/>
+  <dimension ref="A1:E20"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E20" activeCellId="0" sqref="E20"/>
+      <selection pane="topLeft" activeCell="D20" activeCellId="0" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -478,6 +478,23 @@
         <v>260</v>
       </c>
     </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="2" t="n">
+        <v>43924</v>
+      </c>
+      <c r="B20" s="0" t="n">
+        <v>1095</v>
+      </c>
+      <c r="C20" s="0" t="n">
+        <v>395</v>
+      </c>
+      <c r="D20" s="0" t="n">
+        <v>1592</v>
+      </c>
+      <c r="E20" s="0" t="n">
+        <v>351</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
1) Update to New York State hospitalization data for 4 April 2019.
</commit_message>
<xml_diff>
--- a/data/new_york_state_hospitaliztion_and_discharge.xlsx
+++ b/data/new_york_state_hospitaliztion_and_discharge.xlsx
@@ -147,10 +147,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E20"/>
+  <dimension ref="A1:E21"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D20" activeCellId="0" sqref="D20"/>
+      <selection pane="topLeft" activeCell="D22" activeCellId="0" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -495,6 +495,23 @@
         <v>351</v>
       </c>
     </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="2" t="n">
+        <v>43925</v>
+      </c>
+      <c r="B21" s="0" t="n">
+        <v>574</v>
+      </c>
+      <c r="C21" s="0" t="n">
+        <v>250</v>
+      </c>
+      <c r="D21" s="0" t="n">
+        <v>1709</v>
+      </c>
+      <c r="E21" s="0" t="n">
+        <v>316</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
1) Updated New York State hospitalizations for 6 April and 7 April.
</commit_message>
<xml_diff>
--- a/data/new_york_state_hospitaliztion_and_discharge.xlsx
+++ b/data/new_york_state_hospitaliztion_and_discharge.xlsx
@@ -31,10 +31,10 @@
     <t xml:space="preserve">ICU</t>
   </si>
   <si>
-    <t xml:space="preserve">Discharged</t>
+    <t xml:space="preserve">Intubations</t>
   </si>
   <si>
-    <t xml:space="preserve">Intubations</t>
+    <t xml:space="preserve">Discharged</t>
   </si>
 </sst>
 </file>
@@ -147,10 +147,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E21"/>
+  <dimension ref="A1:E23"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D22" activeCellId="0" sqref="D22"/>
+      <selection pane="topLeft" activeCell="E24" activeCellId="0" sqref="E24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -185,7 +185,7 @@
       <c r="C2" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="D2" s="0" t="n">
+      <c r="E2" s="0" t="n">
         <v>0</v>
       </c>
     </row>
@@ -200,10 +200,10 @@
         <v>46</v>
       </c>
       <c r="D3" s="0" t="n">
+        <v>43</v>
+      </c>
+      <c r="E3" s="0" t="n">
         <v>0</v>
-      </c>
-      <c r="E3" s="0" t="n">
-        <v>43</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -217,10 +217,10 @@
         <v>33</v>
       </c>
       <c r="D4" s="0" t="n">
+        <v>27</v>
+      </c>
+      <c r="E4" s="0" t="n">
         <v>123</v>
-      </c>
-      <c r="E4" s="0" t="n">
-        <v>27</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -234,10 +234,10 @@
         <v>104</v>
       </c>
       <c r="D5" s="0" t="n">
+        <v>93</v>
+      </c>
+      <c r="E5" s="0" t="n">
         <v>78</v>
-      </c>
-      <c r="E5" s="0" t="n">
-        <v>93</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -251,10 +251,10 @@
         <v>77</v>
       </c>
       <c r="D6" s="0" t="n">
+        <v>69</v>
+      </c>
+      <c r="E6" s="0" t="n">
         <v>102</v>
-      </c>
-      <c r="E6" s="0" t="n">
-        <v>69</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -268,10 +268,10 @@
         <v>143</v>
       </c>
       <c r="D7" s="0" t="n">
+        <v>116</v>
+      </c>
+      <c r="E7" s="0" t="n">
         <v>150</v>
-      </c>
-      <c r="E7" s="0" t="n">
-        <v>116</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -285,10 +285,10 @@
         <v>140</v>
       </c>
       <c r="D8" s="0" t="n">
+        <v>124</v>
+      </c>
+      <c r="E8" s="0" t="n">
         <v>145</v>
-      </c>
-      <c r="E8" s="0" t="n">
-        <v>124</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -302,10 +302,10 @@
         <v>135</v>
       </c>
       <c r="D9" s="0" t="n">
+        <v>121</v>
+      </c>
+      <c r="E9" s="0" t="n">
         <v>150</v>
-      </c>
-      <c r="E9" s="0" t="n">
-        <v>121</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -319,10 +319,10 @@
         <v>215</v>
       </c>
       <c r="D10" s="0" t="n">
+        <v>192</v>
+      </c>
+      <c r="E10" s="0" t="n">
         <v>278</v>
-      </c>
-      <c r="E10" s="0" t="n">
-        <v>192</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -336,10 +336,10 @@
         <v>192</v>
       </c>
       <c r="D11" s="0" t="n">
+        <v>222</v>
+      </c>
+      <c r="E11" s="0" t="n">
         <v>450</v>
-      </c>
-      <c r="E11" s="0" t="n">
-        <v>222</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -353,10 +353,10 @@
         <v>374</v>
       </c>
       <c r="D12" s="0" t="n">
+        <v>290</v>
+      </c>
+      <c r="E12" s="0" t="n">
         <v>528</v>
-      </c>
-      <c r="E12" s="0" t="n">
-        <v>290</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -370,10 +370,10 @@
         <v>172</v>
       </c>
       <c r="D13" s="0" t="n">
+        <v>200</v>
+      </c>
+      <c r="E13" s="0" t="n">
         <v>681</v>
-      </c>
-      <c r="E13" s="0" t="n">
-        <v>200</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -387,10 +387,10 @@
         <v>282</v>
       </c>
       <c r="D14" s="0" t="n">
+        <v>165</v>
+      </c>
+      <c r="E14" s="0" t="n">
         <v>846</v>
-      </c>
-      <c r="E14" s="0" t="n">
-        <v>165</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -404,10 +404,10 @@
         <v>315</v>
       </c>
       <c r="D15" s="0" t="n">
+        <v>303</v>
+      </c>
+      <c r="E15" s="0" t="n">
         <v>632</v>
-      </c>
-      <c r="E15" s="0" t="n">
-        <v>303</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -421,10 +421,10 @@
         <v>358</v>
       </c>
       <c r="D16" s="0" t="n">
+        <v>295</v>
+      </c>
+      <c r="E16" s="0" t="n">
         <v>771</v>
-      </c>
-      <c r="E16" s="0" t="n">
-        <v>295</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -438,10 +438,10 @@
         <v>312</v>
       </c>
       <c r="D17" s="0" t="n">
+        <v>291</v>
+      </c>
+      <c r="E17" s="0" t="n">
         <v>1167</v>
-      </c>
-      <c r="E17" s="0" t="n">
-        <v>291</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -455,10 +455,10 @@
         <v>374</v>
       </c>
       <c r="D18" s="0" t="n">
+        <v>313</v>
+      </c>
+      <c r="E18" s="0" t="n">
         <v>1292</v>
-      </c>
-      <c r="E18" s="0" t="n">
-        <v>313</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -472,10 +472,10 @@
         <v>335</v>
       </c>
       <c r="D19" s="0" t="n">
+        <v>260</v>
+      </c>
+      <c r="E19" s="0" t="n">
         <v>1452</v>
-      </c>
-      <c r="E19" s="0" t="n">
-        <v>260</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -489,10 +489,10 @@
         <v>395</v>
       </c>
       <c r="D20" s="0" t="n">
+        <v>351</v>
+      </c>
+      <c r="E20" s="0" t="n">
         <v>1592</v>
-      </c>
-      <c r="E20" s="0" t="n">
-        <v>351</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -506,10 +506,44 @@
         <v>250</v>
       </c>
       <c r="D21" s="0" t="n">
+        <v>316</v>
+      </c>
+      <c r="E21" s="0" t="n">
         <v>1709</v>
       </c>
-      <c r="E21" s="0" t="n">
-        <v>316</v>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="2" t="n">
+        <v>43926</v>
+      </c>
+      <c r="B22" s="0" t="n">
+        <v>358</v>
+      </c>
+      <c r="C22" s="0" t="n">
+        <v>128</v>
+      </c>
+      <c r="D22" s="0" t="n">
+        <v>132</v>
+      </c>
+      <c r="E22" s="0" t="n">
+        <v>1179</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="2" t="n">
+        <v>43927</v>
+      </c>
+      <c r="B23" s="0" t="n">
+        <v>656</v>
+      </c>
+      <c r="C23" s="0" t="n">
+        <v>89</v>
+      </c>
+      <c r="D23" s="0" t="n">
+        <v>69</v>
+      </c>
+      <c r="E23" s="0" t="n">
+        <v>1224</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
1) Updated New York State hospitalization data. 2) Added FIPS conversion spreadsheets. 3) Added IHME peak projections by state. 4) Additional analysis of supply chain risk.
</commit_message>
<xml_diff>
--- a/data/new_york_state_hospitaliztion_and_discharge.xlsx
+++ b/data/new_york_state_hospitaliztion_and_discharge.xlsx
@@ -147,10 +147,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E23"/>
+  <dimension ref="A1:E24"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E24" activeCellId="0" sqref="E24"/>
+      <selection pane="topLeft" activeCell="C24" activeCellId="0" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -546,6 +546,14 @@
         <v>1224</v>
       </c>
     </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="2" t="n">
+        <v>43928</v>
+      </c>
+      <c r="B24" s="0" t="n">
+        <v>586</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
1) Added New York state hospitalization data for 9 April 2020.
</commit_message>
<xml_diff>
--- a/data/new_york_state_hospitaliztion_and_discharge.xlsx
+++ b/data/new_york_state_hospitaliztion_and_discharge.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="995" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
@@ -147,15 +147,15 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E24"/>
+  <dimension ref="A1:E25"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C24" activeCellId="0" sqref="C24"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E24" activeCellId="0" sqref="E24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="11.52"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.780612244898"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -537,7 +537,7 @@
         <v>656</v>
       </c>
       <c r="C23" s="0" t="n">
-        <v>89</v>
+        <v>35</v>
       </c>
       <c r="D23" s="0" t="n">
         <v>69</v>
@@ -553,11 +553,31 @@
       <c r="B24" s="0" t="n">
         <v>586</v>
       </c>
+      <c r="C24" s="0" t="n">
+        <v>302</v>
+      </c>
+      <c r="D24" s="0" t="n">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="2" t="n">
+        <v>43929</v>
+      </c>
+      <c r="B25" s="0" t="n">
+        <v>200</v>
+      </c>
+      <c r="C25" s="0" t="n">
+        <v>84</v>
+      </c>
+      <c r="D25" s="0" t="n">
+        <v>88</v>
+      </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>

</xml_diff>

<commit_message>
1) Updated New York state hospitalization data for 9 April 2020. 2) Updated supply chain risk analysis.
</commit_message>
<xml_diff>
--- a/data/new_york_state_hospitaliztion_and_discharge.xlsx
+++ b/data/new_york_state_hospitaliztion_and_discharge.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="995" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t xml:space="preserve">Date</t>
   </si>
@@ -35,6 +35,9 @@
   </si>
   <si>
     <t xml:space="preserve">Discharged</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Deaths</t>
   </si>
 </sst>
 </file>
@@ -147,15 +150,15 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E25"/>
+  <dimension ref="A1:F26"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="E24" activeCellId="0" sqref="E24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8"/>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.780612244898"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="11.78"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -174,6 +177,9 @@
       <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="n">
@@ -511,6 +517,9 @@
       <c r="E21" s="0" t="n">
         <v>1709</v>
       </c>
+      <c r="F21" s="0" t="n">
+        <v>594</v>
+      </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="2" t="n">
@@ -528,6 +537,9 @@
       <c r="E22" s="0" t="n">
         <v>1179</v>
       </c>
+      <c r="F22" s="0" t="n">
+        <v>599</v>
+      </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="2" t="n">
@@ -545,6 +557,9 @@
       <c r="E23" s="0" t="n">
         <v>1224</v>
       </c>
+      <c r="F23" s="0" t="n">
+        <v>731</v>
+      </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="2" t="n">
@@ -559,6 +574,9 @@
       <c r="D24" s="0" t="n">
         <v>94</v>
       </c>
+      <c r="F24" s="0" t="n">
+        <v>779</v>
+      </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="2" t="n">
@@ -573,11 +591,31 @@
       <c r="D25" s="0" t="n">
         <v>88</v>
       </c>
+      <c r="F25" s="0" t="n">
+        <v>799</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="2" t="n">
+        <v>43930</v>
+      </c>
+      <c r="B26" s="0" t="n">
+        <v>290</v>
+      </c>
+      <c r="C26" s="0" t="n">
+        <v>-17</v>
+      </c>
+      <c r="D26" s="0" t="n">
+        <v>109</v>
+      </c>
+      <c r="F26" s="0" t="n">
+        <v>777</v>
+      </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>

</xml_diff>

<commit_message>
1) Added New York state hospitalization data for 11 April 2020. Also includes true up of past four days of discharges. 2) Added `us_state_populations.xlsx` for per capita analysis.
</commit_message>
<xml_diff>
--- a/data/new_york_state_hospitaliztion_and_discharge.xlsx
+++ b/data/new_york_state_hospitaliztion_and_discharge.xlsx
@@ -150,10 +150,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F26"/>
+  <dimension ref="A1:F28"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E24" activeCellId="0" sqref="E24"/>
+      <selection pane="topLeft" activeCell="F29" activeCellId="0" sqref="F29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -574,6 +574,9 @@
       <c r="D24" s="0" t="n">
         <v>94</v>
       </c>
+      <c r="E24" s="0" t="n">
+        <v>1763</v>
+      </c>
       <c r="F24" s="0" t="n">
         <v>779</v>
       </c>
@@ -591,6 +594,9 @@
       <c r="D25" s="0" t="n">
         <v>88</v>
       </c>
+      <c r="E25" s="0" t="n">
+        <v>1944</v>
+      </c>
       <c r="F25" s="0" t="n">
         <v>799</v>
       </c>
@@ -608,8 +614,51 @@
       <c r="D26" s="0" t="n">
         <v>109</v>
       </c>
+      <c r="E26" s="0" t="n">
+        <v>1952</v>
+      </c>
       <c r="F26" s="0" t="n">
         <v>777</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="2" t="n">
+        <v>43931</v>
+      </c>
+      <c r="B27" s="0" t="n">
+        <v>85</v>
+      </c>
+      <c r="C27" s="0" t="n">
+        <v>101</v>
+      </c>
+      <c r="D27" s="0" t="n">
+        <v>-26</v>
+      </c>
+      <c r="E27" s="0" t="n">
+        <v>1776</v>
+      </c>
+      <c r="F27" s="0" t="n">
+        <v>783</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="2" t="n">
+        <v>43932</v>
+      </c>
+      <c r="B28" s="0" t="n">
+        <v>53</v>
+      </c>
+      <c r="C28" s="0" t="n">
+        <v>189</v>
+      </c>
+      <c r="D28" s="0" t="n">
+        <v>110</v>
+      </c>
+      <c r="E28" s="0" t="n">
+        <v>1862</v>
+      </c>
+      <c r="F28" s="0" t="n">
+        <v>758</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
1) Rounding out New York state death data.
</commit_message>
<xml_diff>
--- a/data/new_york_state_hospitaliztion_and_discharge.xlsx
+++ b/data/new_york_state_hospitaliztion_and_discharge.xlsx
@@ -153,7 +153,7 @@
   <dimension ref="A1:F28"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F29" activeCellId="0" sqref="F29"/>
+      <selection pane="topLeft" activeCell="F21" activeCellId="0" sqref="F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -194,6 +194,9 @@
       <c r="E2" s="0" t="n">
         <v>0</v>
       </c>
+      <c r="F2" s="0" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="n">
@@ -211,6 +214,9 @@
       <c r="E3" s="0" t="n">
         <v>0</v>
       </c>
+      <c r="F3" s="0" t="n">
+        <v>5</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="2" t="n">
@@ -228,6 +234,9 @@
       <c r="E4" s="0" t="n">
         <v>123</v>
       </c>
+      <c r="F4" s="0" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="2" t="n">
@@ -245,6 +254,9 @@
       <c r="E5" s="0" t="n">
         <v>78</v>
       </c>
+      <c r="F5" s="0" t="n">
+        <v>23</v>
+      </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="2" t="n">
@@ -262,6 +274,9 @@
       <c r="E6" s="0" t="n">
         <v>102</v>
       </c>
+      <c r="F6" s="0" t="n">
+        <v>9</v>
+      </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="2" t="n">
@@ -279,6 +294,9 @@
       <c r="E7" s="0" t="n">
         <v>150</v>
       </c>
+      <c r="F7" s="0" t="n">
+        <v>70</v>
+      </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="2" t="n">
@@ -296,6 +314,9 @@
       <c r="E8" s="0" t="n">
         <v>145</v>
       </c>
+      <c r="F8" s="0" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="2" t="n">
@@ -313,6 +334,9 @@
       <c r="E9" s="0" t="n">
         <v>150</v>
       </c>
+      <c r="F9" s="0" t="n">
+        <v>96</v>
+      </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="2" t="n">
@@ -330,6 +354,9 @@
       <c r="E10" s="0" t="n">
         <v>278</v>
       </c>
+      <c r="F10" s="0" t="n">
+        <v>75</v>
+      </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="2" t="n">
@@ -347,6 +374,9 @@
       <c r="E11" s="0" t="n">
         <v>450</v>
       </c>
+      <c r="F11" s="0" t="n">
+        <v>100</v>
+      </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="2" t="n">
@@ -364,6 +394,9 @@
       <c r="E12" s="0" t="n">
         <v>528</v>
       </c>
+      <c r="F12" s="0" t="n">
+        <v>134</v>
+      </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="2" t="n">
@@ -381,6 +414,9 @@
       <c r="E13" s="0" t="n">
         <v>681</v>
       </c>
+      <c r="F13" s="0" t="n">
+        <v>209</v>
+      </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="2" t="n">
@@ -398,6 +434,9 @@
       <c r="E14" s="0" t="n">
         <v>846</v>
       </c>
+      <c r="F14" s="0" t="n">
+        <v>237</v>
+      </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="2" t="n">
@@ -415,6 +454,9 @@
       <c r="E15" s="0" t="n">
         <v>632</v>
       </c>
+      <c r="F15" s="0" t="n">
+        <v>253</v>
+      </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="2" t="n">
@@ -432,6 +474,9 @@
       <c r="E16" s="0" t="n">
         <v>771</v>
       </c>
+      <c r="F16" s="0" t="n">
+        <v>332</v>
+      </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="2" t="n">
@@ -449,6 +494,9 @@
       <c r="E17" s="0" t="n">
         <v>1167</v>
       </c>
+      <c r="F17" s="0" t="n">
+        <v>391</v>
+      </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="2" t="n">
@@ -466,6 +514,9 @@
       <c r="E18" s="0" t="n">
         <v>1292</v>
       </c>
+      <c r="F18" s="0" t="n">
+        <v>432</v>
+      </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="2" t="n">
@@ -483,6 +534,9 @@
       <c r="E19" s="0" t="n">
         <v>1452</v>
       </c>
+      <c r="F19" s="0" t="n">
+        <v>562</v>
+      </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="2" t="n">
@@ -499,6 +553,9 @@
       </c>
       <c r="E20" s="0" t="n">
         <v>1592</v>
+      </c>
+      <c r="F20" s="0" t="n">
+        <v>630</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
1) Added New York state hospitalization data for 10 April 2020. Includes new column for New COVID Hospitalizations - think that is the actual number now.
</commit_message>
<xml_diff>
--- a/data/new_york_state_hospitaliztion_and_discharge.xlsx
+++ b/data/new_york_state_hospitaliztion_and_discharge.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t xml:space="preserve">Date</t>
   </si>
@@ -38,6 +38,9 @@
   </si>
   <si>
     <t xml:space="preserve">Deaths</t>
+  </si>
+  <si>
+    <t xml:space="preserve">New COVID Hospitalizations</t>
   </si>
 </sst>
 </file>
@@ -150,15 +153,17 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F28"/>
+  <dimension ref="A1:G29"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F21" activeCellId="0" sqref="F21"/>
+      <selection pane="topLeft" activeCell="G30" activeCellId="0" sqref="G30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="11.78"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="1" style="0" width="11.78"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="24.73"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="8" style="0" width="11.78"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -180,6 +185,9 @@
       <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="n">
@@ -277,6 +285,9 @@
       <c r="F6" s="0" t="n">
         <v>9</v>
       </c>
+      <c r="G6" s="0" t="n">
+        <v>489</v>
+      </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="2" t="n">
@@ -297,6 +308,9 @@
       <c r="F7" s="0" t="n">
         <v>70</v>
       </c>
+      <c r="G7" s="0" t="n">
+        <v>823</v>
+      </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="2" t="n">
@@ -317,6 +331,9 @@
       <c r="F8" s="0" t="n">
         <v>0</v>
       </c>
+      <c r="G8" s="0" t="n">
+        <v>776</v>
+      </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="2" t="n">
@@ -337,6 +354,9 @@
       <c r="F9" s="0" t="n">
         <v>96</v>
       </c>
+      <c r="G9" s="0" t="n">
+        <v>909</v>
+      </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="2" t="n">
@@ -357,6 +377,9 @@
       <c r="F10" s="0" t="n">
         <v>75</v>
       </c>
+      <c r="G10" s="0" t="n">
+        <v>1084</v>
+      </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="2" t="n">
@@ -377,6 +400,9 @@
       <c r="F11" s="0" t="n">
         <v>100</v>
       </c>
+      <c r="G11" s="0" t="n">
+        <v>1796</v>
+      </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="2" t="n">
@@ -397,6 +423,9 @@
       <c r="F12" s="0" t="n">
         <v>134</v>
       </c>
+      <c r="G12" s="0" t="n">
+        <v>1813</v>
+      </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="2" t="n">
@@ -417,6 +446,9 @@
       <c r="F13" s="0" t="n">
         <v>209</v>
       </c>
+      <c r="G13" s="0" t="n">
+        <v>1722</v>
+      </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="2" t="n">
@@ -437,6 +469,9 @@
       <c r="F14" s="0" t="n">
         <v>237</v>
       </c>
+      <c r="G14" s="0" t="n">
+        <v>2241</v>
+      </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="2" t="n">
@@ -457,6 +492,9 @@
       <c r="F15" s="0" t="n">
         <v>253</v>
       </c>
+      <c r="G15" s="0" t="n">
+        <v>1883</v>
+      </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="2" t="n">
@@ -477,6 +515,9 @@
       <c r="F16" s="0" t="n">
         <v>332</v>
       </c>
+      <c r="G16" s="0" t="n">
+        <v>2507</v>
+      </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="2" t="n">
@@ -497,6 +538,9 @@
       <c r="F17" s="0" t="n">
         <v>391</v>
       </c>
+      <c r="G17" s="0" t="n">
+        <v>2844</v>
+      </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="2" t="n">
@@ -517,6 +561,9 @@
       <c r="F18" s="0" t="n">
         <v>432</v>
       </c>
+      <c r="G18" s="0" t="n">
+        <v>2857</v>
+      </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="2" t="n">
@@ -537,6 +584,9 @@
       <c r="F19" s="0" t="n">
         <v>562</v>
       </c>
+      <c r="G19" s="0" t="n">
+        <v>3413</v>
+      </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="2" t="n">
@@ -557,6 +607,9 @@
       <c r="F20" s="0" t="n">
         <v>630</v>
       </c>
+      <c r="G20" s="0" t="n">
+        <v>3261</v>
+      </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="2" t="n">
@@ -577,6 +630,9 @@
       <c r="F21" s="0" t="n">
         <v>594</v>
       </c>
+      <c r="G21" s="0" t="n">
+        <v>2821</v>
+      </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="2" t="n">
@@ -597,6 +653,9 @@
       <c r="F22" s="0" t="n">
         <v>599</v>
       </c>
+      <c r="G22" s="0" t="n">
+        <v>2082</v>
+      </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="2" t="n">
@@ -617,6 +676,9 @@
       <c r="F23" s="0" t="n">
         <v>731</v>
       </c>
+      <c r="G23" s="0" t="n">
+        <v>2553</v>
+      </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="2" t="n">
@@ -637,6 +699,9 @@
       <c r="F24" s="0" t="n">
         <v>779</v>
       </c>
+      <c r="G24" s="0" t="n">
+        <v>3034</v>
+      </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="2" t="n">
@@ -657,6 +722,9 @@
       <c r="F25" s="0" t="n">
         <v>799</v>
       </c>
+      <c r="G25" s="0" t="n">
+        <v>2848</v>
+      </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="2" t="n">
@@ -677,6 +745,9 @@
       <c r="F26" s="0" t="n">
         <v>777</v>
       </c>
+      <c r="G26" s="0" t="n">
+        <v>2882</v>
+      </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="2" t="n">
@@ -697,6 +768,9 @@
       <c r="F27" s="0" t="n">
         <v>783</v>
       </c>
+      <c r="G27" s="0" t="n">
+        <v>2486</v>
+      </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="2" t="n">
@@ -716,6 +790,29 @@
       </c>
       <c r="F28" s="0" t="n">
         <v>758</v>
+      </c>
+      <c r="G28" s="0" t="n">
+        <v>2538</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="2" t="n">
+        <v>43933</v>
+      </c>
+      <c r="B29" s="0" t="n">
+        <v>118</v>
+      </c>
+      <c r="C29" s="0" t="n">
+        <v>-42</v>
+      </c>
+      <c r="D29" s="0" t="n">
+        <v>-21</v>
+      </c>
+      <c r="F29" s="0" t="n">
+        <v>671</v>
+      </c>
+      <c r="G29" s="0" t="n">
+        <v>1958</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
1) Added New York state hospitalization data for 13 April 2020.
</commit_message>
<xml_diff>
--- a/data/new_york_state_hospitaliztion_and_discharge.xlsx
+++ b/data/new_york_state_hospitaliztion_and_discharge.xlsx
@@ -153,10 +153,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G29"/>
+  <dimension ref="A1:G30"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G30" activeCellId="0" sqref="G30"/>
+      <selection pane="topLeft" activeCell="E30" activeCellId="0" sqref="E30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -815,6 +815,26 @@
         <v>1958</v>
       </c>
     </row>
+    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="2" t="n">
+        <v>43934</v>
+      </c>
+      <c r="B30" s="0" t="n">
+        <v>-128</v>
+      </c>
+      <c r="C30" s="0" t="n">
+        <v>69</v>
+      </c>
+      <c r="D30" s="0" t="n">
+        <v>-14</v>
+      </c>
+      <c r="F30" s="0" t="n">
+        <v>778</v>
+      </c>
+      <c r="G30" s="0" t="n">
+        <v>1649</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
1) Added New York state hospitalization data for 14 April 2020.
</commit_message>
<xml_diff>
--- a/data/new_york_state_hospitaliztion_and_discharge.xlsx
+++ b/data/new_york_state_hospitaliztion_and_discharge.xlsx
@@ -153,10 +153,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G30"/>
+  <dimension ref="A1:G31"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E30" activeCellId="0" sqref="E30"/>
+      <selection pane="topLeft" activeCell="F32" activeCellId="0" sqref="F32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -835,6 +835,26 @@
         <v>1649</v>
       </c>
     </row>
+    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="2" t="n">
+        <v>43935</v>
+      </c>
+      <c r="B31" s="0" t="n">
+        <v>-362</v>
+      </c>
+      <c r="C31" s="0" t="n">
+        <v>-20</v>
+      </c>
+      <c r="D31" s="0" t="n">
+        <v>-7</v>
+      </c>
+      <c r="F31" s="0" t="n">
+        <v>752</v>
+      </c>
+      <c r="G31" s="0" t="n">
+        <v>2253</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
1) Adding New York state hospitalization data for 15 April 2020.
</commit_message>
<xml_diff>
--- a/data/new_york_state_hospitaliztion_and_discharge.xlsx
+++ b/data/new_york_state_hospitaliztion_and_discharge.xlsx
@@ -153,10 +153,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G31"/>
+  <dimension ref="A1:G32"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F32" activeCellId="0" sqref="F32"/>
+      <selection pane="topLeft" activeCell="F33" activeCellId="0" sqref="F33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -855,6 +855,26 @@
         <v>2253</v>
       </c>
     </row>
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="2" t="n">
+        <v>43936</v>
+      </c>
+      <c r="B32" s="0" t="n">
+        <v>-606</v>
+      </c>
+      <c r="C32" s="0" t="n">
+        <v>-154</v>
+      </c>
+      <c r="D32" s="0" t="n">
+        <v>-62</v>
+      </c>
+      <c r="F32" s="0" t="n">
+        <v>606</v>
+      </c>
+      <c r="G32" s="0" t="n">
+        <v>1996</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
1) Corrected New York state hospitalization data for 15 April 2020.
</commit_message>
<xml_diff>
--- a/data/new_york_state_hospitaliztion_and_discharge.xlsx
+++ b/data/new_york_state_hospitaliztion_and_discharge.xlsx
@@ -156,7 +156,7 @@
   <dimension ref="A1:G32"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F33" activeCellId="0" sqref="F33"/>
+      <selection pane="topLeft" activeCell="D32" activeCellId="0" sqref="D32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -860,13 +860,13 @@
         <v>43936</v>
       </c>
       <c r="B32" s="0" t="n">
-        <v>-606</v>
+        <v>-600</v>
       </c>
       <c r="C32" s="0" t="n">
-        <v>-154</v>
+        <v>-134</v>
       </c>
       <c r="D32" s="0" t="n">
-        <v>-62</v>
+        <v>-40</v>
       </c>
       <c r="F32" s="0" t="n">
         <v>606</v>

</xml_diff>

<commit_message>
1) Added New York state hospitalization data for 16 April 2020.
</commit_message>
<xml_diff>
--- a/data/new_york_state_hospitaliztion_and_discharge.xlsx
+++ b/data/new_york_state_hospitaliztion_and_discharge.xlsx
@@ -153,10 +153,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G32"/>
+  <dimension ref="A1:G33"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D32" activeCellId="0" sqref="D32"/>
+      <selection pane="topLeft" activeCell="F34" activeCellId="0" sqref="F34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -875,6 +875,26 @@
         <v>1996</v>
       </c>
     </row>
+    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="2" t="n">
+        <v>43937</v>
+      </c>
+      <c r="B33" s="0" t="n">
+        <v>-419</v>
+      </c>
+      <c r="C33" s="0" t="n">
+        <v>-32</v>
+      </c>
+      <c r="D33" s="0" t="n">
+        <v>-73</v>
+      </c>
+      <c r="F33" s="0" t="n">
+        <v>630</v>
+      </c>
+      <c r="G33" s="0" t="n">
+        <v>1974</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
Added New York state hospitalization data for 18 April 2020.
</commit_message>
<xml_diff>
--- a/data/new_york_state_hospitaliztion_and_discharge.xlsx
+++ b/data/new_york_state_hospitaliztion_and_discharge.xlsx
@@ -153,10 +153,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G34"/>
+  <dimension ref="A1:G35"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F35" activeCellId="0" sqref="F35"/>
+      <selection pane="topLeft" activeCell="F36" activeCellId="0" sqref="F36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -915,6 +915,23 @@
         <v>1915</v>
       </c>
     </row>
+    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="2" t="n">
+        <v>43939</v>
+      </c>
+      <c r="B35" s="0" t="n">
+        <v>-754</v>
+      </c>
+      <c r="D35" s="0" t="n">
+        <v>-112</v>
+      </c>
+      <c r="F35" s="0" t="n">
+        <v>507</v>
+      </c>
+      <c r="G35" s="0" t="n">
+        <v>1384</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
1) Adding New York state hospitalization data for 20 April 2020.
</commit_message>
<xml_diff>
--- a/data/new_york_state_hospitaliztion_and_discharge.xlsx
+++ b/data/new_york_state_hospitaliztion_and_discharge.xlsx
@@ -153,10 +153,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G35"/>
+  <dimension ref="A1:G37"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F36" activeCellId="0" sqref="F36"/>
+      <selection pane="topLeft" activeCell="F38" activeCellId="0" sqref="F38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -929,7 +929,41 @@
         <v>507</v>
       </c>
       <c r="G35" s="0" t="n">
-        <v>1384</v>
+        <v>1758</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="2" t="n">
+        <v>43940</v>
+      </c>
+      <c r="B36" s="0" t="n">
+        <v>-404</v>
+      </c>
+      <c r="D36" s="0" t="n">
+        <v>-32</v>
+      </c>
+      <c r="F36" s="0" t="n">
+        <v>478</v>
+      </c>
+      <c r="G36" s="0" t="n">
+        <v>1560</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="2" t="n">
+        <v>43941</v>
+      </c>
+      <c r="B37" s="0" t="n">
+        <v>-27</v>
+      </c>
+      <c r="D37" s="0" t="n">
+        <v>-127</v>
+      </c>
+      <c r="F37" s="0" t="n">
+        <v>481</v>
+      </c>
+      <c r="G37" s="0" t="n">
+        <v>1308</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
1) Added New York state hospitalization data for 21 April 2020.
</commit_message>
<xml_diff>
--- a/data/new_york_state_hospitaliztion_and_discharge.xlsx
+++ b/data/new_york_state_hospitaliztion_and_discharge.xlsx
@@ -153,10 +153,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G37"/>
+  <dimension ref="A1:G38"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F38" activeCellId="0" sqref="F38"/>
+      <selection pane="topLeft" activeCell="F39" activeCellId="0" sqref="F39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -966,6 +966,23 @@
         <v>1308</v>
       </c>
     </row>
+    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="2" t="n">
+        <v>43942</v>
+      </c>
+      <c r="B38" s="0" t="n">
+        <v>-536</v>
+      </c>
+      <c r="D38" s="0" t="n">
+        <v>-41</v>
+      </c>
+      <c r="F38" s="0" t="n">
+        <v>474</v>
+      </c>
+      <c r="G38" s="0" t="n">
+        <v>1366</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
1) Adding New York state hospitalization data for 22 April 2020.
</commit_message>
<xml_diff>
--- a/data/new_york_state_hospitaliztion_and_discharge.xlsx
+++ b/data/new_york_state_hospitaliztion_and_discharge.xlsx
@@ -153,10 +153,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G38"/>
+  <dimension ref="A1:G39"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F39" activeCellId="0" sqref="F39"/>
+      <selection pane="topLeft" activeCell="F40" activeCellId="0" sqref="F40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -983,6 +983,23 @@
         <v>1366</v>
       </c>
     </row>
+    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="2" t="n">
+        <v>43943</v>
+      </c>
+      <c r="B39" s="0" t="n">
+        <v>-578</v>
+      </c>
+      <c r="D39" s="0" t="n">
+        <v>-16</v>
+      </c>
+      <c r="F39" s="0" t="n">
+        <v>438</v>
+      </c>
+      <c r="G39" s="0" t="n">
+        <v>1359</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
1) Updated New York state hospitalization data 24 April 2020.
</commit_message>
<xml_diff>
--- a/data/new_york_state_hospitaliztion_and_discharge.xlsx
+++ b/data/new_york_state_hospitaliztion_and_discharge.xlsx
@@ -153,10 +153,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G39"/>
+  <dimension ref="A1:G41"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F40" activeCellId="0" sqref="F40"/>
+      <selection pane="topLeft" activeCell="F42" activeCellId="0" sqref="F42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1000,6 +1000,40 @@
         <v>1359</v>
       </c>
     </row>
+    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="2" t="n">
+        <v>43944</v>
+      </c>
+      <c r="B40" s="0" t="n">
+        <v>-763</v>
+      </c>
+      <c r="D40" s="0" t="n">
+        <v>-118</v>
+      </c>
+      <c r="F40" s="0" t="n">
+        <v>422</v>
+      </c>
+      <c r="G40" s="0" t="n">
+        <v>1296</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="2" t="n">
+        <v>43945</v>
+      </c>
+      <c r="B41" s="0" t="n">
+        <v>-754</v>
+      </c>
+      <c r="D41" s="0" t="n">
+        <v>-108</v>
+      </c>
+      <c r="F41" s="0" t="n">
+        <v>437</v>
+      </c>
+      <c r="G41" s="0" t="n">
+        <v>1184</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>